<commit_message>
Modify 1900-02-29 handling and fix subsecond rounding (fixes #14)
</commit_message>
<xml_diff>
--- a/tests/testthat/1900.xlsx
+++ b/tests/testthat/1900.xlsx
@@ -49,10 +49,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,10 +355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -376,6 +377,11 @@
         <v>35981</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>